<commit_message>
Main and Spider modification
The program is fully functioning now. It first extracts the title and article URL from the company specific page and then using a callback function it goes one layer deep to open the article url to fetch the date/time and the full text of the articles.
</commit_message>
<xml_diff>
--- a/worklog.xlsx
+++ b/worklog.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E1D6921-61C1-4EFF-A375-3353CECB8B5E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53173504-0392-4184-89C1-D42869C16B7C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Day</t>
   </si>
@@ -29,19 +29,46 @@
   </si>
   <si>
     <t>Work Done</t>
+  </si>
+  <si>
+    <t>Basic spider built that crawls https://economictimes.indiatimes.com . It looks for news title, url, time/date and article in the company specific section of the website. It then saves this datato a csv file after cleaning the string a little bit.</t>
+  </si>
+  <si>
+    <t>Goal for tomorrow</t>
+  </si>
+  <si>
+    <t>Lines of Code</t>
+  </si>
+  <si>
+    <t>Studied the process of crawling data from any webpage, watched python tutorials, built a basic web-scraper by following a youtube tutorial.</t>
+  </si>
+  <si>
+    <t>To Build a basic web scraper that scrapes data of one company from one website and start working from there.</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF586069"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -64,9 +91,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -347,38 +391,89 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="57.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="2" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="2"/>
+    <col min="7" max="7" width="22.42578125" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B3" s="3">
+        <v>43635</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3">
         <v>43636</v>
       </c>
+      <c r="C4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C5" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modified Pipeline, Main, Sub-folders
Updatelog:
Main - removed commandline execution and added script execution of spider
Pipeline - Started using pipeline for csv export
shifted news_spider/news_spider to news_spider
</commit_message>
<xml_diff>
--- a/worklog.xlsx
+++ b/worklog.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53173504-0392-4184-89C1-D42869C16B7C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A6251F-764F-42E6-8B12-40EDF9EF2799}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Day</t>
   </si>
@@ -34,15 +34,9 @@
     <t>Basic spider built that crawls https://economictimes.indiatimes.com . It looks for news title, url, time/date and article in the company specific section of the website. It then saves this datato a csv file after cleaning the string a little bit.</t>
   </si>
   <si>
-    <t>Goal for tomorrow</t>
-  </si>
-  <si>
     <t>Lines of Code</t>
   </si>
   <si>
-    <t>Studied the process of crawling data from any webpage, watched python tutorials, built a basic web-scraper by following a youtube tutorial.</t>
-  </si>
-  <si>
     <t>To Build a basic web scraper that scrapes data of one company from one website and start working from there.</t>
   </si>
   <si>
@@ -50,13 +44,31 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Clean article data in csv file. Include more companies and a new website.</t>
+  </si>
+  <si>
+    <t>Studied the process of crawling data from any webpage, watched python tutorials, built a basic web-scraper by following a youtube tutorial. Reviewed Early Warning Systems (EWS) and understood the flow of the model.</t>
+  </si>
+  <si>
+    <t>Secondary Goals</t>
+  </si>
+  <si>
+    <t>Tomorrow</t>
+  </si>
+  <si>
+    <t>Primary Goals</t>
+  </si>
+  <si>
+    <t>Build keywords dictionary for good and bad metrics</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,13 +82,27 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -91,25 +117,40 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -391,88 +432,119 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="2"/>
-    <col min="7" max="7" width="22.42578125" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="23.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" style="10" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5">
+        <v>43635</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="4">
+        <v>210</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="11"/>
+    </row>
+    <row r="5" spans="1:7" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>2</v>
+      </c>
+      <c r="B5" s="5">
+        <v>43636</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="4">
+        <v>885</v>
+      </c>
+      <c r="E5" s="4">
+        <v>170</v>
+      </c>
+      <c r="F5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="1"/>
+      <c r="G5" s="11" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3">
-        <v>43635</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" s="3">
-        <v>43636</v>
-      </c>
-      <c r="C4" s="5" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
         <v>3</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C5" s="6"/>
+      <c r="B6" s="5">
+        <v>43637</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="11"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Modified input, final output, removed garbage nexturls
Input is now taken from the input.csv file which contains a list of companies in the first column.
Output now also includes the companyname tag
</commit_message>
<xml_diff>
--- a/worklog.xlsx
+++ b/worklog.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02128A51-F424-4BD1-B943-BACD10B9DCE7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C32F887E-F7A3-49B4-A538-F52AB2D3DB5E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Day</t>
   </si>
@@ -53,6 +53,13 @@
   </si>
   <si>
     <t>Project Tracking - Bulk News Crawling and Analysis for EWS</t>
+  </si>
+  <si>
+    <t>Fixed buggy scraping of pages where source code of the site does not load. Cleaned scraped text data (date,time and article). document and add comments to the code.
+keep code in PEP-8 format.</t>
+  </si>
+  <si>
+    <t>Code works for only one company at a time</t>
   </si>
 </sst>
 </file>
@@ -96,7 +103,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -118,6 +125,9 @@
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -402,7 +412,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,77 +449,91 @@
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
     </row>
-    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>1</v>
+      </c>
+      <c r="B5" s="7">
+        <v>43635</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="6"/>
+    </row>
+    <row r="6" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B6" s="7">
-        <v>43635</v>
+        <v>43636</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
         <v>3</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="6"/>
-    </row>
-    <row r="7" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
-        <v>2</v>
-      </c>
       <c r="B7" s="7">
-        <v>43636</v>
+        <v>43637</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
         <v>4</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
-        <v>3</v>
-      </c>
       <c r="B8" s="7">
-        <v>43637</v>
+        <v>43638</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B9" s="7">
-        <v>43638</v>
+        <v>43639</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B10" s="7">
-        <v>43639</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>9</v>
+        <v>43640</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B11" s="7">
-        <v>43640</v>
+        <v>43641</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
keywords counting, Input and output in csv
built input.csv file to take in company name and keywords as input and store the output of keyword count in front of company name
</commit_message>
<xml_diff>
--- a/worklog.xlsx
+++ b/worklog.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C32F887E-F7A3-49B4-A538-F52AB2D3DB5E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB94FCB3-47AF-4CF5-BCA5-7AD3CF67F92B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Day</t>
   </si>
@@ -60,6 +60,18 @@
   </si>
   <si>
     <t>Code works for only one company at a time</t>
+  </si>
+  <si>
+    <t>Spider now accepts input from a csv file that contains a list of companies to be crawled. Modified spider to get stockname from title of company page. Then used nsepy library to get stock info.</t>
+  </si>
+  <si>
+    <t>Company names need to be a perfect match. Improper company names will be skipped.</t>
+  </si>
+  <si>
+    <t>built input.csv file to take in company name and keywords as input and store the output of keyword count in front of company name</t>
+  </si>
+  <si>
+    <t>company names and keywords both need to be a perfect match. Improper company names will be skipped and mismatch keywords wont be counted</t>
   </si>
 </sst>
 </file>
@@ -409,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,12 +540,32 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>7</v>
       </c>
       <c r="B11" s="7">
         <v>43641</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>8</v>
+      </c>
+      <c r="B12" s="7">
+        <v>43642</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
scrape.exe and analyse.exe working
modified scrape.spec to make it work
</commit_message>
<xml_diff>
--- a/worklog.xlsx
+++ b/worklog.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22D39566-DC17-4C08-B96B-7D7B58ADF623}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67FD3565-E023-4722-B6EF-3B7B17D7C738}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Day</t>
   </si>
@@ -75,6 +75,12 @@
   </si>
   <si>
     <t>Fixed company match case. From and to date article filter. Threshold value for matchcase. Company not found update.</t>
+  </si>
+  <si>
+    <t>keyword matching using nltk. created a log for keywords found with article link and company name. pip freeze clean requirements.txt file.</t>
+  </si>
+  <si>
+    <t>Try converting .py to .exe</t>
   </si>
 </sst>
 </file>
@@ -426,8 +432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,7 +609,7 @@
         <v>43646</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>13</v>
       </c>
@@ -614,30 +620,39 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>14</v>
       </c>
       <c r="B18" s="7">
         <v>43648</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>15</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="7">
+        <v>43649</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>18</v>
       </c>

</xml_diff>